<commit_message>
Adding data to keep all members updated with most recent data formatting updates
</commit_message>
<xml_diff>
--- a/Data/Bus_Loads.xlsx
+++ b/Data/Bus_Loads.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JakeLaptop\Documents\GitHub\454_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JakeLaptop\Documents\GitHub\454_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADDD23F0-A9C2-4A02-8E5A-765528FEAC7A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E5B6EF-5A92-4F8E-B48B-762E0ABD4D90}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{E740E765-D248-44F0-B435-17971A0DB4E8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" activeTab="1" xr2:uid="{E740E765-D248-44F0-B435-17971A0DB4E8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Bus Load" sheetId="1" r:id="rId1"/>
+    <sheet name="TestSheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -27,6 +28,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Tstt</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,7 +387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F9784A-855C-4F49-8F42-5E191C723A00}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -457,4 +466,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD144BD4-B26C-4127-9C98-D13598F832D3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added comments in Data_Input, and cleaned up code format, as well as added both admittance matrices for reference. Admittance matrix csv files cannot be open when trying to run code
</commit_message>
<xml_diff>
--- a/Data/Bus_Loads.xlsx
+++ b/Data/Bus_Loads.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JakeLaptop\Documents\GitHub\454_Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JakeDesktop\Documents\Git\454_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E5B6EF-5A92-4F8E-B48B-762E0ABD4D90}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5631057B-848C-48C5-86C3-F79FF998E2BE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" activeTab="1" xr2:uid="{E740E765-D248-44F0-B435-17971A0DB4E8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{E740E765-D248-44F0-B435-17971A0DB4E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Load" sheetId="1" r:id="rId1"/>
-    <sheet name="TestSheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,14 +27,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Tstt</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,7 +378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F9784A-855C-4F49-8F42-5E191C723A00}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -466,22 +457,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD144BD4-B26C-4127-9C98-D13598F832D3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>